<commit_message>
removed excess columns in dtr summary and added legends to per employee report
</commit_message>
<xml_diff>
--- a/exceltocsv/public/reports/employee dtr/"Gatan, Jr.",Mario Haris.xlsx
+++ b/exceltocsv/public/reports/employee dtr/"Gatan, Jr.",Mario Haris.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="68" xml:space="preserve">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="72" xml:space="preserve">
   <si>
     <t>iRipple, Inc.</t>
   </si>
@@ -194,15 +194,25 @@
     <t>ACCUMULATED OT</t>
   </si>
   <si>
+    <t>Legends:</t>
+  </si>
+  <si>
     <t>LATES</t>
   </si>
   <si>
+    <t>Employee has request(s)/remark(s) for that day.
+*May incur late and/or undertime depending on his or her time-in and time-out.</t>
+  </si>
+  <si>
     <t>ACCUMULATED VL</t>
   </si>
   <si>
     <t>ACCUMULATED SL</t>
   </si>
   <si>
+    <t>Employee is considered half-day because of his time-in or time-out.</t>
+  </si>
+  <si>
     <t>VL BALANCE</t>
   </si>
   <si>
@@ -210,6 +220,9 @@
   </si>
   <si>
     <t>SL BALANCE</t>
+  </si>
+  <si>
+    <t>Employee has no time-in and therefore, considered as absent.</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -223,7 +236,7 @@
     <numFmt numFmtId="100" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="101" formatCode="yyyy/mm/dd hh:mm:ss"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <name val="Arial"/>
       <sz val="11"/>
@@ -266,9 +279,16 @@
       <name val="Arial"/>
       <sz val="11"/>
       <family val="1"/>
+      <b val="true"/>
+      <u val="true"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="11"/>
+      <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,6 +310,21 @@
         <fgColor rgb="FFDF5E5E"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF29A3CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC66"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDF5E5E"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border/>
@@ -395,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="1" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="0" numFmtId="14" fontId="0" fillId="0" xfId="0" applyNumberFormat="1"/>
@@ -415,7 +450,11 @@
     <xf borderId="6" numFmtId="0" fontId="6" fillId="4" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf borderId="7" numFmtId="0" fontId="7" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf borderId="0" numFmtId="0" fontId="0" fillId="5" applyNumberFormat="false" applyFill="true" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="0" numFmtId="0" fontId="0" fillId="6" applyNumberFormat="false" applyFill="true" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="0" numFmtId="0" fontId="0" fillId="7" applyNumberFormat="false" applyFill="true" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="0" numFmtId="0" fontId="7" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="7" numFmtId="0" fontId="8" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -640,12 +679,12 @@
       <c r="E8" s="7" t="n">
         <v>1.0</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="7" t="n">
+        <v>2.75</v>
+      </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="7" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
@@ -678,7 +717,9 @@
       <c r="E9" s="5" t="n">
         <v>0.75</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5" t="n">
+        <v>2.0</v>
+      </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
@@ -711,9 +752,7 @@
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
-      <c r="I10" s="8" t="n">
-        <v>1</v>
-      </c>
+      <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
@@ -901,9 +940,7 @@
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
-      <c r="I16" s="8" t="n">
-        <v>1</v>
-      </c>
+      <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
@@ -993,16 +1030,16 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="9" t="s">
+      <c r="B19" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>56</v>
       </c>
       <c r="E19" s="5" t="str">
@@ -1043,16 +1080,16 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="9" t="s">
+      <c r="B20" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="13" t="s">
         <v>56</v>
       </c>
       <c r="E20" s="5" t="str">
@@ -1093,22 +1130,22 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="9" t="s">
+      <c r="B21" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="13" t="s">
         <v>56</v>
       </c>
       <c r="G21" s="5" t="str">
@@ -1143,25 +1180,25 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G22" s="9" t="s">
+      <c r="B22" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="13" t="s">
         <v>56</v>
       </c>
       <c r="H22" s="5" t="str">
@@ -1194,10 +1231,10 @@
     </row>
     <row r="23"/>
     <row r="24">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="13" t="s">
         <v>56</v>
       </c>
       <c r="C24" s="5" t="str">
@@ -1206,40 +1243,40 @@
       <c r="D24" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="J24" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="K24" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="L24" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="M24" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="N24" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="O24" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="P24" s="0" t="s">
+      <c r="E24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="O24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P24" s="3" t="s">
         <v>56</v>
       </c>
       <c r="Q24" s="0" t="str">
@@ -1259,10 +1296,10 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="9" t="s">
+      <c r="A25" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="13" t="s">
         <v>56</v>
       </c>
       <c r="C25" s="5" t="str">
@@ -1271,40 +1308,40 @@
       <c r="D25" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="G25" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="I25" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="J25" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="K25" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="L25" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="M25" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="N25" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="O25" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="P25" s="0" t="s">
+      <c r="E25" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="J25" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="K25" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="L25" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="M25" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="N25" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="O25" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="P25" s="12" t="s">
         <v>56</v>
       </c>
       <c r="Q25" s="0" t="str">
@@ -1324,10 +1361,10 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" s="9" t="s">
+      <c r="A26" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="13" t="s">
         <v>56</v>
       </c>
       <c r="C26" s="5" t="str">
@@ -1336,40 +1373,40 @@
       <c r="D26" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E26" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="I26" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="J26" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="K26" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="L26" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="M26" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="N26" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="O26" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="P26" s="0" t="s">
+      <c r="E26" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="K26" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="L26" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="M26" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="N26" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="O26" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="P26" s="12" t="s">
         <v>56</v>
       </c>
       <c r="Q26" s="0" t="str">
@@ -1389,10 +1426,10 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="9" t="s">
+      <c r="A27" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="13" t="s">
         <v>56</v>
       </c>
       <c r="C27" s="5" t="str">
@@ -1401,40 +1438,40 @@
       <c r="D27" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="J27" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="K27" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="L27" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="M27" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="N27" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="O27" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="P27" s="0" t="s">
+      <c r="E27" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="I27" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="K27" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="L27" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="M27" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="N27" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="O27" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="P27" s="12" t="s">
         <v>56</v>
       </c>
       <c r="Q27" s="0" t="str">
@@ -1454,52 +1491,52 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B28" s="9" t="s">
+      <c r="A28" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="13" t="s">
         <v>56</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E28" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="I28" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="J28" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="K28" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="L28" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="M28" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="N28" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="O28" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="P28" s="0" t="s">
+      <c r="E28" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="I28" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="K28" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="L28" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="M28" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="N28" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="O28" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="P28" s="12" t="s">
         <v>56</v>
       </c>
       <c r="Q28" s="0" t="str">
@@ -1519,52 +1556,52 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B29" s="9" t="s">
+      <c r="A29" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="13" t="s">
         <v>56</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E29" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="G29" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="H29" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="I29" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="J29" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="K29" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="L29" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="M29" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="N29" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="O29" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="P29" s="0" t="s">
+      <c r="E29" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="K29" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="L29" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="M29" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="N29" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="O29" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="P29" s="12" t="s">
         <v>56</v>
       </c>
       <c r="Q29" s="0" t="str">
@@ -1584,10 +1621,10 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" s="9" t="s">
+      <c r="A30" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="13" t="s">
         <v>56</v>
       </c>
       <c r="C30" s="5" t="str">
@@ -1596,40 +1633,40 @@
       <c r="D30" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E30" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F30" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="I30" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="J30" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="K30" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="L30" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="M30" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="N30" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="O30" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="P30" s="0" t="s">
+      <c r="E30" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="K30" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="L30" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="M30" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="N30" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="O30" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="P30" s="12" t="s">
         <v>56</v>
       </c>
       <c r="Q30" s="0" t="str">
@@ -1638,7 +1675,7 @@
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
-  <mergeCells count="18">
+  <mergeCells count="25">
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="A2:P2"/>
     <mergeCell ref="A3:P3"/>
@@ -1651,11 +1688,18 @@
     <mergeCell ref="A22:G22"/>
     <mergeCell ref="J22:P22"/>
     <mergeCell ref="A24:B24"/>
+    <mergeCell ref="E24:P24"/>
     <mergeCell ref="A25:B25"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:P26"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:P28"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:P30"/>
     <mergeCell ref="A30:B30"/>
   </mergeCells>
   <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>

</xml_diff>